<commit_message>
Modification du fichier execl
</commit_message>
<xml_diff>
--- a/fichierExcel.xlsx
+++ b/fichierExcel.xlsx
@@ -26,7 +26,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
   <si>
-    <t>Bonjour le monde !</t>
+    <t>Temouafo defo boris</t>
   </si>
 </sst>
 </file>
@@ -347,7 +347,7 @@
   <dimension ref="A2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
troisième commit du clone
</commit_message>
<xml_diff>
--- a/fichierExcel.xlsx
+++ b/fichierExcel.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CloneDevoir\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dossier_devoir\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -26,7 +26,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
   <si>
-    <t>Hello world !</t>
+    <t>Temouafo defo boris</t>
   </si>
 </sst>
 </file>
@@ -347,7 +347,7 @@
   <dimension ref="A2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>